<commit_message>
user registration last update
</commit_message>
<xml_diff>
--- a/Test Cases Template Search Page.xlsx
+++ b/Test Cases Template Search Page.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgyurov\Desktop\PetStoreTestingTask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzhingova\Desktop\PetStoreTestingTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -707,22 +707,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">This TC will show that the Search option is working correctly when the User type a Keyword and Pet Breed and option from Pet Type and Subscription
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Checking the search form with User typing a Keyword and selecting "Pet Breed" and  an option from "Pet Type" and "Subscription"</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">This TC will show that the Search option is working correctly when the User type Keyword and Pet Birthday and option from Pet Type and Subscription
 </t>
     </r>
@@ -844,9 +828,6 @@
     <t>A window with "you have successfully searched by: Pet Birthday"</t>
   </si>
   <si>
-    <t>A window with "you have successfully searched by: Pet Owner's name"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">This TC will show that Search option is working with "User's Town" and "Pet Owner's name"checkbox are checked 
 </t>
@@ -2877,7 +2858,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> Pet Breed checkbox
+      <t xml:space="preserve"> Pet Birthday checkbox
 4.</t>
     </r>
     <r>
@@ -2960,162 +2941,53 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>1. Navigate to Search page
+    <t>Search Page</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: User's Town and Pet Type"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: User's Town and Subscription"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: Pet Owner's name and Pet Type"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: Pet Owner's name and Subscription"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: Pet Breed and Pet Type"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: Pet Breed and Subscription"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: Pet Birthday and Pet Type"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by: Pet Birthday and Subscription"</t>
+  </si>
+  <si>
+    <t>A window with "you have successfully searched by:   User's Town and Pet Owner's name"</t>
+  </si>
+  <si>
+    <t>This TC will show that the Search option is working correctly when the User type a Keyword and Pet Breed and option from Pet Type and Subscription
+Checking the search form with User typing a Keyword and selecting "Pet Breed" and  an option from "Pet Type" and "Subscription"</t>
+  </si>
+  <si>
+    <t>1. Navigate to Search page
 2.In search field enter Keyword
-3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Select</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Check</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> Pet Birthday checkbox
-4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Select</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Check</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> option from Pet type
-3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Select</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Check</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> option fromSubscription
+3.Select Check Pet Breed checkbox
+4.Select Check option from Pet type
+3.Select Check option fromSubscription
 4.Press Search option</t>
-    </r>
-  </si>
-  <si>
-    <t>Search Page</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: User's Town and Pet Type"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: User's Town and Subscription"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: Pet Owner's name and Pet Type"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: Pet Owner's name and Subscription"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: Pet Breed and Pet Type"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: Pet Breed and Subscription"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: Pet Birthday and Pet Type"</t>
-  </si>
-  <si>
-    <t>A window with "you have successfully searched by: Pet Birthday and Subscription"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3181,8 +3053,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3214,6 +3093,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -3265,13 +3149,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3288,18 +3173,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3308,9 +3181,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3324,9 +3194,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3336,6 +3203,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3343,8 +3222,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3651,509 +3531,511 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="22.7109375" style="11" customWidth="1"/>
+    <col min="7" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:14" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>121</v>
+      <c r="D3" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>122</v>
+      <c r="F3" s="12" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="100.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="100.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+    </row>
+    <row r="6" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>148</v>
+        <v>126</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-    </row>
-    <row r="7" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>150</v>
+        <v>125</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="F7" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>151</v>
+        <v>124</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>152</v>
+        <v>127</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="F9" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>153</v>
+        <v>128</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>78</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>154</v>
+        <v>129</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="F11" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="229.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>155</v>
+        <v>130</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>153</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="F12" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>156</v>
+        <v>131</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="F13" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>157</v>
+        <v>132</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="F14" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>158</v>
+        <v>133</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>180</v>
+      <c r="F15" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:14" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:14" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>159</v>
+        <v>134</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="F16" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="F17" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E18" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="F18" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="F19" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E20" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="F20" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="267.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E23" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="F23" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="267.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E24" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="F24" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -4162,18 +4044,18 @@
       <c r="C25" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="15" t="s">
+      <c r="D25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="F25" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -4182,18 +4064,18 @@
       <c r="C26" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E26" s="15" t="s">
+      <c r="D26" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="F26" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="293.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -4202,18 +4084,18 @@
       <c r="C27" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E27" s="15" t="s">
+      <c r="D27" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="F27" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="318.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -4222,155 +4104,155 @@
       <c r="C28" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="E28" s="15" t="s">
+      <c r="D28" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="F28" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E29" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="I29" s="21"/>
-    </row>
-    <row r="30" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="F29" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E30" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="17" t="s">
-        <v>146</v>
+      <c r="F30" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="H31"/>
-    </row>
-    <row r="32" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20" t="s">
+      <c r="C35" s="13"/>
+      <c r="D35" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20" t="s">
+      <c r="C36" s="13"/>
+      <c r="D36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="13" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>